<commit_message>
Agregados comentarios y se quitaron los datos harcodeados
</commit_message>
<xml_diff>
--- a/datos de prueba.xlsx
+++ b/datos de prueba.xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{54EB99E9-30AB-46BA-95C7-CCE8875CB952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Academia\xForce\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E8D2E12-C1CC-4375-A780-BDF72C57CABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="14835" windowHeight="11475" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3090" yWindow="1815" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="users and pass" sheetId="1" r:id="rId1"/>
@@ -16,23 +21,11 @@
     <sheet name="Sheet2" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:M9"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="125">
   <si>
     <t>xforce1</t>
   </si>
@@ -387,6 +380,36 @@
   </si>
   <si>
     <t>Permitir regresarse y seguir comprando antes de pagar</t>
+  </si>
+  <si>
+    <t>Luis Fernando Diaz</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Aguascalientes</t>
+  </si>
+  <si>
+    <t>Jose Juan Vazquez</t>
+  </si>
+  <si>
+    <t>4573123447582740</t>
+  </si>
+  <si>
+    <t>4573123447583445</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>2024</t>
+  </si>
+  <si>
+    <t>2025</t>
   </si>
 </sst>
 </file>
@@ -459,7 +482,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -469,6 +492,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -784,33 +808,73 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
+      <c r="C2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>124</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -818,7 +882,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A38E1128-EADC-402D-B03C-15E350D6CBE2}">
   <dimension ref="B1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -1420,12 +1484,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BAE9EC29EFF9BD498F24B0A00A7BA695" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="207590255b200e05398b58740b949ddf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e9e42d1e-f44a-4146-b7e9-87d8ba66eaa3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="02d1540dd62600fd625a946b9579a99b" ns2:_="">
     <xsd:import namespace="e9e42d1e-f44a-4146-b7e9-87d8ba66eaa3"/>
@@ -1595,6 +1653,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E694AA5-CB02-4C0C-A115-23098F8987D4}">
   <ds:schemaRefs>
@@ -1604,15 +1668,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27150A1E-25EB-4F12-ACD4-7C31B981E5A8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EC5ED2C-C035-462C-B79A-BB31AC046B2D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1628,4 +1683,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27150A1E-25EB-4F12-ACD4-7C31B981E5A8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>